<commit_message>
fix lỗi và làm nút down file
</commit_message>
<xml_diff>
--- a/Uploads/Test.xlsx
+++ b/Uploads/Test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F0CB441-A726-4543-B00A-F22F53B27670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39770C8D-5984-4852-84C5-69E45F124683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{312F7849-C732-4D77-A136-BA2C873C6A55}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>EMAIL</t>
   </si>
@@ -46,97 +46,94 @@
     <t>TEAM</t>
   </si>
   <si>
+    <t>hung.197pm21929@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Thế Quang</t>
+  </si>
+  <si>
+    <t>duong.197pm21908@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hoai.197pm21924@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>dat.197pm09430@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thao.187pm20578@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>loi.197pm09475@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>nhan.197pm21962@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thinh.197pm21987@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>bao.197pm21895@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hoang.197pm21925@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>trang.197pm31214@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>khoi.197pm21939@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thuy.197pm21989@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>quang.197pm31195@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>duy.197pm21905@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>tuan.197pm31224@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>thien.197pm21985@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>truong.197pm21993@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>hieu.197pm21922@vanlanguni.vn</t>
+  </si>
+  <si>
+    <t>Nguyễn Minh Tân</t>
+  </si>
+  <si>
+    <t>hiếu</t>
+  </si>
+  <si>
+    <t>dung.197pm31142@vanlangu</t>
+  </si>
+  <si>
+    <t>phong.197pm31190@vanla</t>
+  </si>
+  <si>
+    <t>dat.197pm31149@vanlan</t>
+  </si>
+  <si>
     <t>TOPIC</t>
   </si>
   <si>
-    <t>CUSTOMER</t>
-  </si>
-  <si>
-    <t>hung.197pm21929@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>Nguyễn Thế Quang</t>
-  </si>
-  <si>
-    <t>duong.197pm21908@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>hoai.197pm21924@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>dat.197pm09430@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>thao.187pm20578@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>loi.197pm09475@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>nhan.197pm21962@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>thinh.197pm21987@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>bao.197pm21895@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>hoang.197pm21925@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>trang.197pm31214@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>khoi.197pm21939@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>thuy.197pm21989@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>quang.197pm31195@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>duy.197pm21905@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>tuan.197pm31224@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>thien.197pm21985@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>truong.197pm21993@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>hieu.197pm21922@vanlanguni.vn</t>
-  </si>
-  <si>
-    <t>Nguyễn Minh Tân</t>
-  </si>
-  <si>
-    <t>hiếu</t>
-  </si>
-  <si>
-    <t>Đề tài 03: WEBSITE QUẢN LÝ NHÀ HÀNG</t>
-  </si>
-  <si>
-    <t>Đề tài 20: WEBSITE BÁN LAPTOP</t>
-  </si>
-  <si>
-    <t>Đề tài 04: ỨNG DỤNG ĐIỆN THOẠI TRA CỨU VÉ MÁY BAY</t>
-  </si>
-  <si>
-    <t>Đề tài 01: WEBSITE BÁN VÀNG</t>
-  </si>
-  <si>
-    <t>dung.197pm31142@vanlangu</t>
-  </si>
-  <si>
-    <t>phong.197pm31190@vanla</t>
-  </si>
-  <si>
-    <t>dat.197pm31149@vanlan</t>
+    <t>Đề tài 01: WEBSITE BÁN NHÀ</t>
+  </si>
+  <si>
+    <t>Đề tài 20: WEBSITE XE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đề tài 03: WEBSITE QUẢN LÝ HỌC SINH </t>
+  </si>
+  <si>
+    <t>Đề tài 04: ỨNG DỤNG ĐIỆN THOẠI TRA CỨU KẾT QUẢ HỌC TẬP</t>
   </si>
 </sst>
 </file>
@@ -184,12 +181,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -197,6 +188,12 @@
       <family val="2"/>
       <charset val="163"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -375,7 +372,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -406,6 +403,18 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -415,26 +424,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -751,22 +748,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B10CCD1-A6C9-4FE1-A309-C960A450BB88}">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.19921875" customWidth="1"/>
-    <col min="3" max="3" width="55.59765625" customWidth="1"/>
-    <col min="4" max="4" width="20.296875" customWidth="1"/>
-    <col min="5" max="5" width="20.796875" customWidth="1"/>
+    <col min="2" max="2" width="27.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="71.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -774,277 +770,238 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="12"/>
+      <c r="B4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="12"/>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="13"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+    </row>
+    <row r="8" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="15"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="18"/>
+      <c r="D10" s="15"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="18"/>
+      <c r="D11" s="15"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="18"/>
+      <c r="D12" s="15"/>
+    </row>
+    <row r="13" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="13"/>
+      <c r="B13" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:4" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="11">
+        <v>3</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="12"/>
+      <c r="B16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="12"/>
+      <c r="B17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
+      <c r="B18" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+    </row>
+    <row r="19" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="13"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="13">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
-      <c r="B3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="15"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="17"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
-      <c r="B12" s="19" t="s">
+      <c r="B20" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-    </row>
-    <row r="13" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="15"/>
-      <c r="B13" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13">
-        <v>3</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="10" t="s">
+      <c r="D20" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="12"/>
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="12"/>
+      <c r="B23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
-      <c r="B17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
-      <c r="B18" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="13">
-        <v>4</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="3" t="s">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="12"/>
+      <c r="B24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
-      <c r="B22" s="3" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+    </row>
+    <row r="25" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="13"/>
+      <c r="B25" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
-      <c r="B23" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
-      <c r="B24" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="1:5" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="12">
     <mergeCell ref="A14:A19"/>
     <mergeCell ref="A20:A25"/>
-    <mergeCell ref="C2:C7"/>
     <mergeCell ref="D2:D7"/>
-    <mergeCell ref="E2:E7"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
+    <mergeCell ref="D8:D13"/>
+    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="D20:D25"/>
+    <mergeCell ref="C2:C7"/>
     <mergeCell ref="C8:C13"/>
-    <mergeCell ref="D8:D13"/>
-    <mergeCell ref="E8:E13"/>
-    <mergeCell ref="E14:E19"/>
-    <mergeCell ref="E20:E25"/>
-    <mergeCell ref="D14:D19"/>
+    <mergeCell ref="C14:C19"/>
     <mergeCell ref="C20:C25"/>
-    <mergeCell ref="D20:D25"/>
-    <mergeCell ref="C14:C19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B11" r:id="rId1" xr:uid="{0F16C281-D07F-458C-96E3-C71F1E8A3F66}"/>

</xml_diff>